<commit_message>
created the full stack implementation of creating a new variable version by uploading an excel file
</commit_message>
<xml_diff>
--- a/target/classes/data/variables/Niguarda_v2.xlsx
+++ b/target/classes/data/variables/Niguarda_v2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="124">
   <si>
     <t xml:space="preserve">csvFile</t>
   </si>
@@ -70,48 +70,63 @@
     <t xml:space="preserve">Patient ID</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/pet/av45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SESSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M,F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender: M/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/root/pet/fdg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA_NASCITA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/root/pet/pib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical_report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/root/brain_anatomy/brainstem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_UNI_NOSOLOGICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinical episode ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">/root/brain_anatomy/tiv</t>
   </si>
   <si>
-    <t xml:space="preserve">SESSO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nominal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M,F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender: M/F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA_NASCITA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of Birth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical_report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_UNI_NOSOLOGICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clinical episode ID</t>
-  </si>
-  <si>
     <t xml:space="preserve">CODICE_PRESTAZIONE_ICD9</t>
   </si>
   <si>
     <t xml:space="preserve">Hospital treatment code (ICD9) for the MRI</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/_3rdventricle</t>
+  </si>
+  <si>
     <t xml:space="preserve">HANDEDNESS</t>
   </si>
   <si>
@@ -124,7 +139,7 @@
     <t xml:space="preserve">1 means R and 2 means L</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/brain_anatomy/brainstem</t>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/_4thventricle</t>
   </si>
   <si>
     <t xml:space="preserve">EDUCATION</t>
@@ -133,13 +148,16 @@
     <t xml:space="preserve">Years of Education</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/csfglobal</t>
+  </si>
+  <si>
     <t xml:space="preserve">PROFILO_CLINICO</t>
   </si>
   <si>
     <t xml:space="preserve">DIAGNOSIS CATEGORY</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/brain_anatomy/csf_volume/_3rdventricle</t>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/leftinflatvent</t>
   </si>
   <si>
     <t xml:space="preserve">MMSE_SCORE</t>
@@ -148,7 +166,7 @@
     <t xml:space="preserve">Mini Mental State Examination (MMSE) total score</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/pet/av45</t>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/leftlateralventricle</t>
   </si>
   <si>
     <t xml:space="preserve">ORIENTATION_TO_TIME</t>
@@ -157,7 +175,7 @@
     <t xml:space="preserve">MMSE subscore for orientation to time</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/pet/fdg</t>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/rightinflatvent</t>
   </si>
   <si>
     <t xml:space="preserve">ORIENTATION_TO_PLACE</t>
@@ -166,7 +184,7 @@
     <t xml:space="preserve">MMSE subscore for orientation to place</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/pet/pib</t>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/rightlateralventricle</t>
   </si>
   <si>
     <t xml:space="preserve">REGISTRATION</t>
@@ -175,24 +193,36 @@
     <t xml:space="preserve">MMSE subscore for registration</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/grey_matter_volume/cerebellum/cerebellarvermallobulesiv</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALCULATION</t>
   </si>
   <si>
     <t xml:space="preserve">MMSE subscore for calculation</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/grey_matter_volume/cerebellum/cerebellarvermallobulesviiix</t>
+  </si>
+  <si>
     <t xml:space="preserve">ATTENTION</t>
   </si>
   <si>
     <t xml:space="preserve">MMSE subscore for attention</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/grey_matter_volume/cerebellum/cerebellarvermallobulesvivii</t>
+  </si>
+  <si>
     <t xml:space="preserve">RECALL</t>
   </si>
   <si>
     <t xml:space="preserve">MMSE subscore for recall</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/grey_matter_volume/cerebellum/leftcerebellumexterior</t>
+  </si>
+  <si>
     <t xml:space="preserve">LANGUAGE</t>
   </si>
   <si>
@@ -343,115 +373,25 @@
     <t xml:space="preserve">sample</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/diagnosis/dataset_specific_diagnosis/PROFILO_CLINICO/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/demographics/handedness</t>
-  </si>
-  <si>
     <t xml:space="preserve">years</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/demographics/EDUCATION</t>
-  </si>
-  <si>
     <t xml:space="preserve">points</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/neuropsychology/minimentalstate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/ORIENTATION_TO_TIME/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/ORIENTATION_TO_PLACE/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/REGISTRATION/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/CALCULATION/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/ATTENTION/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/RECALL/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/LANGUAGE/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/REPETITION/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/STAGE_COMMANDS_3 /</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/READ_AND_OBEY/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/SENTENCE/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/neuropsychology/mmse/PRAXIA/</t>
-  </si>
-  <si>
     <t xml:space="preserve">MRI id</t>
   </si>
   <si>
     <t xml:space="preserve">WARD APPLYING THE EXAM</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/imaging/CODICE_PRESTAZIONE_ICD9/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date of the MRI</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/imaging/DATA_ESAME/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/imaging/RICHIEDENTE/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Way to perform hospitalization ( 1 =inpatient surgery 2=day hospital 4= MAC 5= anticipato).</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/clinical/REGIME/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/REPARTO_INIZIO/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/REPARTO_FINE/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/diagnosis/COD_DIAGNOSI_ICD9/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/diagnosis/CODICE_DIAGNOSI_1_ICD9/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/diagnosis/CODICE_DIAGNOSI_2_ICD9/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/diagnosis/CODICE_DIAGNOSI_3_ICD9/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/diagnosis/CODICE_DIAGNOSI_4_ICD9/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/diagnosis/CODICE_DIAGNOSI_5_ICD9/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/diagnosis/CODICE_DIAGNOSI_6_ICD9/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Episode type (“I” = inpatient “U” =emergency “E” = outpatient)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/root/clinical/TIPO_EPISODIO/</t>
   </si>
 </sst>
 </file>
@@ -560,7 +500,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -597,10 +537,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -621,13 +557,16 @@
   <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+      <selection pane="topLeft" activeCell="N78" activeCellId="0" sqref="N78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,7 +649,7 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,26 +657,26 @@
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
@@ -756,19 +695,19 @@
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="0" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -776,64 +715,67 @@
         <v>14</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="0" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I7" s="4"/>
+      <c r="J7" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
@@ -843,41 +785,41 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="0" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
@@ -887,19 +829,19 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
@@ -909,19 +851,19 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="0" t="s">
-        <v>45</v>
+      <c r="J12" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
@@ -931,19 +873,19 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
@@ -953,19 +895,19 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="0" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
@@ -975,19 +917,19 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="0" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
@@ -997,19 +939,19 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="0" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
@@ -1019,19 +961,19 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="0" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
@@ -1041,19 +983,19 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="0" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
@@ -1063,19 +1005,19 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="0" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
@@ -1085,19 +1027,19 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
@@ -1107,19 +1049,19 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="0" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
@@ -1129,19 +1071,19 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
@@ -1151,16 +1093,16 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="0" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>12</v>
@@ -1178,19 +1120,19 @@
         <v>15</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1198,198 +1140,198 @@
         <v>14</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>16</v>
+        <v>86</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J34" s="0" t="s">
         <v>16</v>
@@ -1397,100 +1339,100 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="8" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1498,22 +1440,22 @@
         <v>14</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -1521,22 +1463,22 @@
         <v>14</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -1544,561 +1486,561 @@
         <v>14</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J44" s="0" t="s">
-        <v>107</v>
+        <v>44</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>115</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>116</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>117</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>119</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>121</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="J60" s="9" t="s">
-        <v>124</v>
+        <v>119</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>130</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>135</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>137</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>139</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>143</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>